<commit_message>
Edycja pliku przykładów; dodanie nowego pliku z moimi raportami
</commit_message>
<xml_diff>
--- a/przykładowy raport defektów QA10 ListBoxer.xlsx
+++ b/przykładowy raport defektów QA10 ListBoxer.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df0caa2c2b2b1609/Desktop/testowanie/GoIt/zad 25-26/LachMal/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_CA4E2B7114127B18627A01D6F4623375695C8B31" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6EABE15-95C5-4FF4-A1F5-06A2EA2B6410}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13890"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raport defektów-testy statycze" sheetId="1" r:id="rId1"/>
@@ -14,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="94">
   <si>
     <t>Strona / Linia / Wymaganie</t>
   </si>
@@ -317,7 +312,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -385,11 +380,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -711,820 +703,767 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="60.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="2"/>
-    <col min="8" max="8" width="36.7109375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="60.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="8" max="8" width="36.6640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" ht="54" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3" t="s">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3" t="s">
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    </row>
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    </row>
+    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    </row>
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    </row>
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3" t="s">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    </row>
+    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    </row>
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    </row>
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3" t="s">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3" t="s">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    </row>
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3" t="s">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3" t="s">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    </row>
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3" t="s">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    </row>
+    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3" t="s">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    </row>
+    <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3" t="s">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    </row>
+    <row r="35" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3" t="s">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    </row>
+    <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3" t="s">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    </row>
+    <row r="37" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3" t="s">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3" t="s">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:8" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3" t="s">
+    </row>
+    <row r="39" spans="1:8" ht="48.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="6" t="s">
+      <c r="H39" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3" t="s">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    </row>
+    <row r="41" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3" t="s">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3" t="s">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3" t="s">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3" t="s">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+    </row>
+    <row r="45" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3" t="s">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3" t="s">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3" t="s">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+    </row>
+    <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3" t="s">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+    </row>
+    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3" t="s">
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3" t="s">
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3" t="s">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3" t="s">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+    </row>
+    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3" t="s">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3" t="s">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="1"/>
-    </row>
-    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="F61" s="2" t="s">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F61" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F62" s="2" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F62" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="F63" s="2" t="s">
+    <row r="63" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F63" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>